<commit_message>
Format ATP7 data presentation
</commit_message>
<xml_diff>
--- a/atp_update/ATP7.xlsx
+++ b/atp_update/ATP7.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="1056" windowWidth="15576" windowHeight="11256"/>
+    <workbookView xWindow="-45" yWindow="1050" windowWidth="15570" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="262">
   <si>
     <t>007-004-00-1</t>
   </si>
@@ -437,13 +437,6 @@
   <si>
     <t>piridabén (ISO);
 2-terc-butil-5-(4-terc-bu­tilbenciltio)-4-cloro­piridazin-3(2H)-ona</t>
-  </si>
-  <si>
-    <t>fenol, dodecil-, ramificado [1];
-fenol, 2-dodecil-, ramificado;
-fenol, 3-dodecil-, ramificado;
-fenol, 4-dodecil-, ramificado;
-fenol, deriYados tetrapropenílicos [2]</t>
   </si>
   <si>
     <t>tembotriona (ISO);
@@ -590,13 +583,6 @@
 Aquatic Chronic 1</t>
   </si>
   <si>
-    <t>Acute Tox. 3
-Acute Tox. 3
-Aquatic Acute 1
-Aquatic Chronic 1
-Eye Irrit. 2</t>
-  </si>
-  <si>
     <t>Skin Corr. 1C
 Aquatic Acute 1
 Aquatic Chronic 1</t>
@@ -743,13 +729,6 @@
 H410</t>
   </si>
   <si>
-    <t>H331
-H301
-H400
-H410
-H319</t>
-  </si>
-  <si>
     <t>H314
 H400
 H410</t>
@@ -757,12 +736,6 @@
   <si>
     <t>H361d
 H373 (ojos, riñones, hígado)
-H317
-H400
-H410</t>
-  </si>
-  <si>
-    <t>H373 (riñones
 H317
 H400
 H410</t>
@@ -902,28 +875,6 @@
     <t>GHS07
 GHS09
 Wng</t>
-  </si>
-  <si>
-    <t>carvona (ISO);
-2-metil-5-(prop-1-en-2-il)ciclohex-2-en-1-ona [1]
-d-carvona;
-(5S)-2-metil-5-(prop-1-en-2-il)ciclohex-2-en-1-ona [2]
-l-carvona;
-(5R)-2-metil-5-(prop-1-en-2-il)ciclohex-2-en-1-ona [3]</t>
-  </si>
-  <si>
-    <t>202-759-5 [1]
-218-827-2 [2]
-229-352-5 [3]</t>
-  </si>
-  <si>
-    <t>99-49-0 [1]
-2244-16-8 [2]
-6485-40-1 [3]</t>
-  </si>
-  <si>
-    <t>121158-58-5 [1]
-74499-35-7 [2]</t>
   </si>
   <si>
     <t>H373
@@ -1064,6 +1015,83 @@
   <si>
     <t>EUH029
 EUH032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H331
+H301
+H400
+H410
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acute Tox. 3
+Acute Tox. 3
+Aquatic Acute 1
+Aquatic Chronic 1
+</t>
+  </si>
+  <si>
+    <t>Eye Irrit. 2</t>
+  </si>
+  <si>
+    <t>H373 (riñones)
+H317
+H400
+H410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fenol, dodecil-, ramificado [1];
+fenol, 2-dodecil-, ramificado;
+fenol, 3-dodecil-, ramificado;
+fenol, 4-dodecil-, ramificado;
+</t>
+  </si>
+  <si>
+    <t>fenol, deriYados tetrapropenílicos [2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121158-58-5 [1]
+</t>
+  </si>
+  <si>
+    <t>74499-35-7 [2]</t>
+  </si>
+  <si>
+    <t>M = 10
+M = 11</t>
+  </si>
+  <si>
+    <t>d-carvona;
+(5S)-2-metil-5-(prop-1-en-2-il)ciclohex-2-en-1-ona [2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carvona (ISO);
+2-metil-5-(prop-1-en-2-il)ciclohex-2-en-1-ona [1]
+</t>
+  </si>
+  <si>
+    <t>l-carvona;
+(5R)-2-metil-5-(prop-1-en-2-il)ciclohex-2-en-1-ona [3]</t>
+  </si>
+  <si>
+    <t>218-827-2 [2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202-759-5 [1]
+</t>
+  </si>
+  <si>
+    <t>229-352-5 [3]</t>
+  </si>
+  <si>
+    <t>2244-16-8 [2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99-49-0 [1]
+</t>
+  </si>
+  <si>
+    <t>6485-40-1 [3]</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1121,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1103,6 +1131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1128,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1158,6 +1192,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1454,31 +1503,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A15" sqref="A15"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="6" customWidth="1"/>
     <col min="12" max="12" width="8" style="6"/>
-    <col min="13" max="16384" width="9.109375" style="6"/>
+    <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="10" customFormat="1" ht="13.8">
+    <row r="1" spans="1:27" s="10" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1529,12 +1578,12 @@
       <c r="Z1" s="9"/>
       <c r="AA1" s="9"/>
     </row>
-    <row r="2" spans="1:27" ht="52.8">
+    <row r="2" spans="1:27" ht="63.75">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -1543,29 +1592,29 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="79.2">
+    <row r="3" spans="1:27" ht="76.5">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1579,26 +1628,26 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:27" ht="52.8">
+    <row r="4" spans="1:27" ht="38.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1612,19 +1661,19 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="105.6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="102">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1638,25 +1687,25 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="105.6">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="102">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1670,19 +1719,19 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="52.8">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="51">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1696,23 +1745,23 @@
         <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:27" ht="52.8">
+    <row r="8" spans="1:27" ht="38.25">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1726,23 +1775,23 @@
         <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:27" ht="39.6">
+    <row r="9" spans="1:27" ht="38.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1756,19 +1805,19 @@
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="66">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="63.75">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1782,23 +1831,23 @@
         <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:27" ht="79.2">
+    <row r="11" spans="1:27" ht="76.5">
       <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1812,26 +1861,26 @@
         <v>37</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:27" ht="66">
+    <row r="12" spans="1:27" ht="63.75">
       <c r="A12" s="7" t="s">
         <v>126</v>
       </c>
@@ -1845,23 +1894,23 @@
         <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:27" ht="66">
+    <row r="13" spans="1:27" ht="63.75">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -1874,24 +1923,24 @@
       <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>167</v>
+      <c r="E13" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:27" ht="26.4">
+    <row r="14" spans="1:27" ht="25.5">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -1904,578 +1953,662 @@
       <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="G14" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="66">
+    <row r="15" spans="1:27" ht="63.75">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:27" s="15" customFormat="1" ht="51.75" customHeight="1">
+      <c r="A16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" ht="51">
+      <c r="A17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="15" customFormat="1" ht="42" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="15" customFormat="1" ht="42" customHeight="1">
+      <c r="A19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="63.75">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="51">
+      <c r="A21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="25.5">
+      <c r="A22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F22" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="38.25">
+      <c r="A23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="25.5">
+      <c r="A24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="76.5">
+      <c r="A25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:27" ht="79.2">
-      <c r="A16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="66">
-      <c r="A17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="G25" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="63.75">
+      <c r="A26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="52.8">
-      <c r="A18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="26.4">
-      <c r="A19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="39.6">
-      <c r="A20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="26.4">
-      <c r="A21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="79.2">
-      <c r="A22" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" ht="66">
-      <c r="A23" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" ht="66">
-      <c r="A24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" ht="66">
-      <c r="A25" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" ht="52.8">
-      <c r="A26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>208</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>245</v>
+        <v>193</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="52.8">
+    <row r="27" spans="1:11" ht="63.75">
       <c r="A27" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" ht="38.25">
+      <c r="A28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="51">
+      <c r="A29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" ht="51">
+      <c r="A30" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="38.25">
+      <c r="A31" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" ht="25.5">
+      <c r="A32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" ht="51">
+      <c r="A33" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="F33" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" ht="51">
+      <c r="A34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="52.8">
-      <c r="A28" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" ht="52.8">
-      <c r="A29" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" ht="52.8">
-      <c r="A30" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="G34" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" ht="25.5">
+      <c r="A35" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="38.25">
+      <c r="A36" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="K30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" ht="52.8">
-      <c r="A31" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" ht="52.8">
-      <c r="A32" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="52.8">
-      <c r="A33" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="B34" s="5"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="5"/>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="B35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="F36" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" s="5"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2489,7 +2622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2501,7 +2634,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>